<commit_message>
Updating Documents according to The last bersions of CYRS & HSI & SRS: - Modifing the PP due to delivery - Modifing the RTM - Updatinhg the logo in all the documents Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ/SIQ_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\SIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37535AB6-91B0-4A3D-83A5-69A62C9BCDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F3A57F-DA86-4AD9-872E-86293289A147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,29 +243,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1171576</xdr:colOff>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2486026</xdr:colOff>
+      <xdr:colOff>3228975</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7026B58A-52F9-45EC-9E84-68C046028813}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{006FFAC4-54F1-410E-959B-1F54D6519349}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -279,8 +279,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1781176" y="19050"/>
-          <a:ext cx="1314450" cy="228600"/>
+          <a:off x="1352550" y="0"/>
+          <a:ext cx="2486025" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="9" t="s">
         <v>0</v>
       </c>

</xml_diff>